<commit_message>
ExampleMapping UserStory01 - Reg
</commit_message>
<xml_diff>
--- a/docs/ExampleMap_TA.xlsx
+++ b/docs/ExampleMap_TA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pocza\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C13E3A2-041F-4AB6-8180-7FA0602EE605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37DAD2C-A5E1-41E6-B5D4-5F1CE54FB1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>This is a rule</t>
   </si>
@@ -491,12 +491,6 @@
 - különböző jelszavak megadása
 =&gt;  Inaktív "Következő" gomb és megjelenik a "A megadott jelszavak nem egyeznek!" hibaüzenet </t>
     </r>
-  </si>
-  <si>
-    <t>tesrtsedfs</t>
-  </si>
-  <si>
-    <t>dfsdfsdf</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1114,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -1151,12 +1145,8 @@
       <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="E2" s="1"/>
+      <c r="G2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="L2" s="1"/>

</xml_diff>

<commit_message>
ExampleMapping UserStory02 - Log
</commit_message>
<xml_diff>
--- a/docs/ExampleMap_TA.xlsx
+++ b/docs/ExampleMap_TA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pocza\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37DAD2C-A5E1-41E6-B5D4-5F1CE54FB1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB654BAB-080F-4E04-A542-1CB8C066330F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regisztracio" sheetId="6" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>This is a rule</t>
   </si>
@@ -491,6 +491,9 @@
 - különböző jelszavak megadása
 =&gt;  Inaktív "Következő" gomb és megjelenik a "A megadott jelszavak nem egyeznek!" hibaüzenet </t>
     </r>
+  </si>
+  <si>
+    <t>Bejelentkezes</t>
   </si>
 </sst>
 </file>
@@ -1113,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BBE0450-19F7-4FBD-B41F-F6A4254C5495}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -1255,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E4351E-459D-4623-B01D-053C343F0B92}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -1283,11 +1286,9 @@
       <c r="A1" s="11"/>
     </row>
     <row r="2" spans="1:14" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="A2"/>
       <c r="C2" s="10" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1"/>
@@ -1298,11 +1299,9 @@
     </row>
     <row r="3" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:14" s="5" customFormat="1" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="9" t="s">
-        <v>0</v>
-      </c>
+      <c r="A4" s="9"/>
       <c r="B4" s="3"/>
-      <c r="C4"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
       <c r="F4" s="3"/>
@@ -1313,11 +1312,9 @@
       <c r="L4" s="4"/>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:14" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="6" t="s">
-        <v>1</v>
-      </c>
+    <row r="5" spans="1:14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" ht="138" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6"/>
       <c r="C6"/>
       <c r="E6" s="1"/>
       <c r="G6" s="1"/>
@@ -1326,7 +1323,7 @@
       <c r="L6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
       <c r="C7" s="1"/>
       <c r="E7" s="1"/>
@@ -1337,9 +1334,7 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="138" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="8" t="s">
-        <v>4</v>
-      </c>
+      <c r="A8"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="14"/>

</xml_diff>